<commit_message>
Added input on hybZono operations difficulty
</commit_message>
<xml_diff>
--- a/Class_Properties_Methods_Map.xlsx
+++ b/Class_Properties_Methods_Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpk170130\Documents\GitHub\Hybrid_Zonotope_Toolbox_alpha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bird6\Documents\GitHub\Hybrid_Zonotope_Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46171A7C-55F1-431A-9864-B969D3AF64E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19FD6E5-325D-436A-ADB8-8D6EBE7D7BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
   <si>
     <t>Class</t>
   </si>
@@ -313,9 +313,6 @@
     <t>compute inner-approximation of set Z</t>
   </si>
   <si>
-    <t>hard?</t>
-  </si>
-  <si>
     <t>convexRelax</t>
   </si>
   <si>
@@ -377,6 +374,21 @@
   </si>
   <si>
     <t>Dependent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intractable </t>
+  </si>
+  <si>
+    <t>exponential growth if set is not convex</t>
+  </si>
+  <si>
+    <t>hard!</t>
+  </si>
+  <si>
+    <t>DNE yet</t>
+  </si>
+  <si>
+    <t>intractable unless Zh - zonotope</t>
   </si>
 </sst>
 </file>
@@ -491,17 +503,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -667,55 +679,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -997,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,21 +975,21 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1041,16 +1004,16 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1066,14 +1029,14 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="O3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="10"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1088,16 +1051,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1108,16 +1071,16 @@
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1128,16 +1091,16 @@
         <v>16</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1148,16 +1111,16 @@
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1168,16 +1131,16 @@
         <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1188,16 +1151,16 @@
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1208,16 +1171,16 @@
         <v>35</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1228,24 +1191,24 @@
         <v>23</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -1260,16 +1223,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="7"/>
     </row>
@@ -1281,16 +1244,16 @@
         <v>24</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1301,16 +1264,16 @@
         <v>27</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1321,16 +1284,16 @@
         <v>29</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,16 +1304,16 @@
         <v>31</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -1379,10 +1342,10 @@
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="10"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1411,7 +1374,7 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1439,7 +1402,7 @@
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1454,7 +1417,7 @@
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1474,10 +1437,10 @@
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="10"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1492,16 +1455,16 @@
         <v>36</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G29" s="7"/>
     </row>
@@ -1513,16 +1476,16 @@
         <v>43</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" s="7"/>
     </row>
@@ -1534,16 +1497,16 @@
         <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G31" s="7"/>
     </row>
@@ -1555,7 +1518,7 @@
         <v>51</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -1593,7 +1556,7 @@
         <v>55</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1618,16 +1581,18 @@
       <c r="B37" t="s">
         <v>72</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="12"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="10"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1659,10 +1624,10 @@
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="12"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="10"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -1688,7 +1653,9 @@
       <c r="B43" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -1719,20 +1686,20 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="12"/>
+      <c r="A47" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="13"/>
       <c r="C47" s="10"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -1741,34 +1708,34 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New functions and MLD example
</commit_message>
<xml_diff>
--- a/Class_Properties_Methods_Map.xlsx
+++ b/Class_Properties_Methods_Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bird6\Documents\GitHub\Hybrid_Zonotope_Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpk170130\Documents\GitHub\Hybrid_Zonotope_Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19FD6E5-325D-436A-ADB8-8D6EBE7D7BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED33B089-156E-4F8C-97AF-5800C356B83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>Koeln, Justin</author>
   </authors>
   <commentList>
-    <comment ref="A42" authorId="0" shapeId="0" xr:uid="{3117F28B-6DDE-4BDB-AAA7-D3DFB36CF6A7}">
+    <comment ref="A44" authorId="0" shapeId="0" xr:uid="{3117F28B-6DDE-4BDB-AAA7-D3DFB36CF6A7}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="119">
   <si>
     <t>Class</t>
   </si>
@@ -217,9 +217,6 @@
     <t>convexHull</t>
   </si>
   <si>
-    <t>generalizedIntersection</t>
-  </si>
-  <si>
     <t>halfspaceIntersection</t>
   </si>
   <si>
@@ -389,13 +386,43 @@
   </si>
   <si>
     <t>intractable unless Zh - zonotope</t>
+  </si>
+  <si>
+    <t>Need to check tolerances</t>
+  </si>
+  <si>
+    <t>Could benefit from multi-solution approach</t>
+  </si>
+  <si>
+    <t>projection on to specified dimensions</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>Auxiliary</t>
+  </si>
+  <si>
+    <t>matchSetType</t>
+  </si>
+  <si>
+    <t>case input objects into matching set types</t>
+  </si>
+  <si>
+    <t>projection</t>
+  </si>
+  <si>
+    <t>stepMLD</t>
+  </si>
+  <si>
+    <t>1-step reachable set for MLD system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,6 +468,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -474,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -509,11 +542,98 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -958,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +1109,7 @@
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -1004,16 +1124,16 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="O2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1029,7 +1149,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="O3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1054,13 +1174,13 @@
         <v>101</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1074,13 +1194,13 @@
         <v>101</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1094,13 +1214,13 @@
         <v>101</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1114,13 +1234,13 @@
         <v>101</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1134,13 +1254,13 @@
         <v>101</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1154,13 +1274,13 @@
         <v>101</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F10" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1174,13 +1294,13 @@
         <v>101</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1194,13 +1314,13 @@
         <v>101</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -1226,13 +1346,13 @@
         <v>101</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" s="7"/>
     </row>
@@ -1247,13 +1367,13 @@
         <v>101</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1267,13 +1387,13 @@
         <v>101</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1287,13 +1407,13 @@
         <v>101</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,13 +1427,13 @@
         <v>101</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -1354,10 +1474,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1367,14 +1487,14 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1382,10 +1502,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1395,14 +1515,14 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1410,14 +1530,14 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1425,13 +1545,15 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1449,223 +1571,266 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>101</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>117</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+        <v>55</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
+      <c r="A38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
+      <c r="A40" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="A41" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
+      <c r="A43" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -1677,80 +1842,180 @@
         <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
+      <c r="A47" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" t="s">
-        <v>88</v>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A28:B28"/>
   </mergeCells>
+  <conditionalFormatting sqref="C22:C27 C30:F34 C36:F36">
+    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
+      <formula>"Dependent"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="46" operator="equal">
+      <formula>"Hidden"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="47" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="48" operator="equal">
+      <formula>"Abstract"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C5:F18">
+    <cfRule type="cellIs" dxfId="31" priority="49" operator="equal">
+      <formula>"Dependent"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="50" operator="equal">
+      <formula>"Hidden"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="51" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="52" operator="equal">
+      <formula>"Abstract"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"Dependent"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"Hidden"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"Abstract"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Dependent"</formula>
     </cfRule>
@@ -1764,7 +2029,7 @@
       <formula>"Abstract"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C27">
+  <conditionalFormatting sqref="F41">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Dependent"</formula>
     </cfRule>
@@ -1778,7 +2043,7 @@
       <formula>"Abstract"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:C31">
+  <conditionalFormatting sqref="C29:F31">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Dependent"</formula>
     </cfRule>
@@ -1792,7 +2057,7 @@
       <formula>"Abstract"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D31">
+  <conditionalFormatting sqref="C55:F55">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Dependent"</formula>
     </cfRule>
@@ -1806,7 +2071,7 @@
       <formula>"Abstract"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E31">
+  <conditionalFormatting sqref="C35">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Dependent"</formula>
     </cfRule>
@@ -1820,7 +2085,7 @@
       <formula>"Abstract"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F31">
+  <conditionalFormatting sqref="D35:F35">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Dependent"</formula>
     </cfRule>
@@ -1835,6 +2100,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>